<commit_message>
Changes 23-10-2023 xlsx file change
</commit_message>
<xml_diff>
--- a/commands-2.xlsx
+++ b/commands-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
+    <workbookView xWindow="4545" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Wedding Timeline Planner" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="103">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -369,12 +369,24 @@
   <si>
     <t>Set Personal or fav command in base_aliases</t>
   </si>
+  <si>
+    <t>Redis Server in installation Process and Steps</t>
+  </si>
+  <si>
+    <t>Search Service in Teminal</t>
+  </si>
+  <si>
+    <t>Restart or Relaod Ngnix server</t>
+  </si>
+  <si>
+    <t>To Check Info short or brief about It's often used for authentication and secure communication between your local machine and GitHub.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,29 +409,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FFE1696C"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1" tint="0.14999847407452621"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -446,30 +437,8 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="5" tint="-9.9978637043366805E-2"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1" tint="0.14999847407452621"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="5" tint="-9.9978637043366805E-2"/>
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -478,13 +447,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -511,16 +473,52 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="28"/>
-      <color rgb="FF0070C0"/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9" tint="-0.499984740745262"/>
+      <color rgb="FF002060"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FF002060"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF002060"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF002060"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color rgb="FF002060"/>
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -637,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,7 +652,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -663,9 +661,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -681,162 +676,168 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,58 +933,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2319130</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>4946787</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>159823</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="Design decoration - floating flowers">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4058478" y="0"/>
-          <a:ext cx="2617304" cy="1133858"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -1259,890 +1208,937 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:I143"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F138" sqref="F138"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="46" customWidth="1"/>
     <col min="3" max="4" width="1.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.5" style="17" customWidth="1"/>
+    <col min="5" max="5" width="1.5" style="15" customWidth="1"/>
     <col min="6" max="6" width="126.625" style="3" customWidth="1"/>
     <col min="7" max="7" width="7.375" style="1" customWidth="1"/>
     <col min="8" max="9" width="1.625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="18"/>
-      <c r="F1" s="13"/>
-      <c r="H1" s="12" t="s">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="44"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="12"/>
+      <c r="H1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="14" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:9" s="13" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="16"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+    </row>
+    <row r="3" spans="1:9" s="13" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="45"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="20"/>
+      <c r="D5" s="18"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="18"/>
       <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
-      <c r="D7" s="20"/>
+      <c r="B7" s="63"/>
+      <c r="D7" s="18"/>
       <c r="F7" s="4"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41" t="s">
+      <c r="B8" s="64"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="42" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="29" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="8"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="42" t="s">
+      <c r="B10" s="66"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="29" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="8"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26" t="s">
         <v>4</v>
       </c>
       <c r="G11" s="8"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
+    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="20"/>
+      <c r="D12" s="18"/>
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="48"/>
+      <c r="D13" s="18"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="F13" s="5" t="s">
+      <c r="D14" s="18"/>
+      <c r="F14" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="F14" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="G14" s="8"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="20"/>
-      <c r="F15" s="25" t="s">
-        <v>11</v>
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="F15" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="G15" s="8"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="20"/>
-      <c r="F16" s="5" t="s">
-        <v>12</v>
+    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="18"/>
+      <c r="F16" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="G16" s="8"/>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="20"/>
-      <c r="F17" s="41" t="s">
-        <v>13</v>
+      <c r="D17" s="18"/>
+      <c r="F17" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="G17" s="8"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="20"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39" t="s">
-        <v>14</v>
+    <row r="18" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="18"/>
+      <c r="F18" s="28" t="s">
+        <v>13</v>
       </c>
       <c r="G18" s="8"/>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="20"/>
-      <c r="F19" s="5"/>
+      <c r="B19" s="50"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="26" t="s">
+        <v>14</v>
+      </c>
       <c r="G19" s="8"/>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
+      <c r="D20" s="18"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="8"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39" t="s">
+      <c r="D21" s="18"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="20"/>
-      <c r="F21" s="5"/>
       <c r="G21" s="8"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="F22" s="43" t="s">
-        <v>17</v>
-      </c>
+    </row>
+    <row r="22" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="18"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="8"/>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="35"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="39" t="s">
-        <v>18</v>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="F23" s="30" t="s">
+        <v>17</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="D24" s="20"/>
-      <c r="F24" s="5"/>
+      <c r="B24" s="68"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26" t="s">
+        <v>18</v>
+      </c>
       <c r="G24" s="8"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="45"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B25" s="52"/>
+      <c r="D25" s="18"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="8"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="45"/>
-      <c r="D26" s="20"/>
+      <c r="B26" s="50"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="20"/>
       <c r="F26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="45"/>
-      <c r="D27" s="20"/>
+      <c r="B27" s="50"/>
+      <c r="D27" s="18"/>
       <c r="F27" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="20"/>
-      <c r="F28" s="5"/>
+      <c r="B28" s="50"/>
+      <c r="D28" s="18"/>
+      <c r="F28" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="G28" s="8"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="45"/>
-      <c r="D29" s="20"/>
-      <c r="F29" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="D29" s="18"/>
+      <c r="F29" s="5"/>
       <c r="G29" s="8"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="45"/>
-      <c r="D30" s="20"/>
+      <c r="B30" s="50"/>
+      <c r="D30" s="18"/>
       <c r="F30" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="45"/>
-      <c r="D31" s="20"/>
+      <c r="B31" s="50"/>
+      <c r="D31" s="18"/>
       <c r="F31" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="48"/>
-      <c r="D32" s="20"/>
-      <c r="F32" s="66" t="s">
+    <row r="32" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="50"/>
+      <c r="D32" s="18"/>
+      <c r="F32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="53"/>
+      <c r="D33" s="18"/>
+      <c r="F33" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="21"/>
-      <c r="D33" s="20"/>
-      <c r="F33" s="65"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="21"/>
-      <c r="D34" s="20"/>
-      <c r="F34" s="67" t="s">
+    <row r="34" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" s="54"/>
+      <c r="D34" s="18"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" s="54"/>
+      <c r="D35" s="18"/>
+      <c r="F35" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35" s="22"/>
-      <c r="D35" s="20"/>
-      <c r="F35" s="65"/>
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="46"/>
-      <c r="D36" s="20"/>
-      <c r="F36" s="5" t="s">
+      <c r="B36" s="55"/>
+      <c r="D36" s="18"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" s="56"/>
+      <c r="D37" s="18"/>
+      <c r="F37" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="G36" s="8"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37" s="46"/>
-      <c r="D37" s="20"/>
-      <c r="F37" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
     <row r="38" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" s="46"/>
-      <c r="D38" s="20"/>
+      <c r="B38" s="56"/>
+      <c r="D38" s="18"/>
       <c r="F38" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
     <row r="39" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39" s="46"/>
-      <c r="D39" s="20"/>
+      <c r="B39" s="56"/>
+      <c r="D39" s="18"/>
       <c r="F39" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-      <c r="D40" s="20"/>
-      <c r="F40" s="5"/>
+    <row r="40" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="56"/>
+      <c r="D40" s="18"/>
+      <c r="F40" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="G40" s="8"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="2:9" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="45"/>
-      <c r="D41" s="20"/>
-      <c r="F41" s="5" t="s">
-        <v>87</v>
-      </c>
+    <row r="41" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="52"/>
+      <c r="D41" s="18"/>
+      <c r="F41" s="5"/>
       <c r="G41" s="8"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="20"/>
-      <c r="F42" s="5"/>
+    <row r="42" spans="2:9" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="50"/>
+      <c r="D42" s="18"/>
+      <c r="F42" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="G42" s="8"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" s="48"/>
-      <c r="D43" s="20"/>
-      <c r="F43" s="5" t="s">
-        <v>59</v>
-      </c>
+    <row r="43" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="18"/>
+      <c r="F43" s="5"/>
       <c r="G43" s="8"/>
       <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
     </row>
     <row r="44" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44" s="47"/>
-      <c r="D44" s="20"/>
-      <c r="F44" s="5"/>
+      <c r="B44" s="53"/>
+      <c r="D44" s="18"/>
+      <c r="F44" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="G44" s="8"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="2:9" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45" s="49"/>
-      <c r="D45" s="50"/>
-      <c r="F45" s="41" t="s">
+    <row r="45" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="57"/>
+      <c r="D45" s="18"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="2:9" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="58"/>
+      <c r="D46" s="31"/>
+      <c r="F46" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="G45" s="51"/>
-      <c r="H45" s="52"/>
-    </row>
-    <row r="46" spans="2:9" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" s="49"/>
-      <c r="D46" s="50"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="52"/>
-    </row>
-    <row r="47" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="44"/>
-      <c r="D47" s="20"/>
-      <c r="F47" s="5" t="s">
+      <c r="G46" s="32"/>
+      <c r="H46" s="33"/>
+    </row>
+    <row r="47" spans="2:9" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" s="58"/>
+      <c r="D47" s="31"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="33"/>
+    </row>
+    <row r="48" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="47"/>
+      <c r="D48" s="18"/>
+      <c r="F48" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="2:9" s="53" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="58"/>
-      <c r="D48" s="54"/>
-      <c r="F48" s="55" t="s">
+      <c r="G48" s="8"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="2:9" s="34" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="50"/>
+      <c r="D49" s="35"/>
+      <c r="F49" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="G48" s="56"/>
-      <c r="H48" s="57"/>
-      <c r="I48" s="57"/>
-    </row>
-    <row r="49" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D49" s="20"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
     </row>
     <row r="50" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="45"/>
-      <c r="D50" s="20"/>
-      <c r="F50" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="D50" s="18"/>
+      <c r="F50" s="5"/>
       <c r="G50" s="8"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
     <row r="51" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="45"/>
-      <c r="D51" s="20"/>
+      <c r="B51" s="50"/>
+      <c r="D51" s="18"/>
       <c r="F51" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
     <row r="52" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="45"/>
-      <c r="D52" s="20"/>
+      <c r="B52" s="50"/>
+      <c r="D52" s="18"/>
       <c r="F52" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G52" s="8"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D53" s="20"/>
-      <c r="F53" s="5"/>
+      <c r="B53" s="50"/>
+      <c r="D53" s="18"/>
+      <c r="F53" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="G53" s="8"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B54" s="46"/>
-      <c r="D54" s="20"/>
-      <c r="F54" s="5" t="s">
-        <v>34</v>
-      </c>
+    <row r="54" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="59"/>
+      <c r="D54" s="18"/>
+      <c r="F54" s="5"/>
       <c r="G54" s="8"/>
       <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="44"/>
-      <c r="D55" s="20"/>
-      <c r="F55" s="5" t="s">
-        <v>35</v>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="18"/>
+      <c r="F55" s="43" t="s">
+        <v>100</v>
       </c>
       <c r="G55" s="8"/>
       <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
     </row>
     <row r="56" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D56" s="20"/>
+      <c r="D56" s="18"/>
       <c r="F56" s="5"/>
       <c r="G56" s="8"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="64"/>
-      <c r="D57" s="20"/>
+    <row r="57" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" s="56"/>
+      <c r="D57" s="18"/>
       <c r="F57" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G57" s="8"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="64"/>
-      <c r="D58" s="20"/>
-      <c r="F58" s="30" t="s">
-        <v>37</v>
+    <row r="58" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="47"/>
+      <c r="D58" s="18"/>
+      <c r="F58" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="45"/>
-      <c r="D59" s="20"/>
-      <c r="F59" s="28" t="s">
+    <row r="59" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="48"/>
+      <c r="D59" s="18"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="47"/>
+      <c r="D60" s="18"/>
+      <c r="F60" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="G60" s="8"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="18"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+    </row>
+    <row r="62" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="50"/>
+      <c r="D62" s="18"/>
+      <c r="F62" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G62" s="8"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="50"/>
+      <c r="D63" s="18"/>
+      <c r="F63" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G63" s="8"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="50"/>
+      <c r="D64" s="18"/>
+      <c r="F64" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G59" s="10"/>
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="45"/>
-      <c r="D60" s="20"/>
-      <c r="F60" s="29" t="s">
+      <c r="G64" s="9"/>
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="50"/>
+      <c r="D65" s="18"/>
+      <c r="F65" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G60" s="11"/>
-    </row>
-    <row r="61" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="45"/>
-      <c r="D61" s="20"/>
-      <c r="F61" s="3" t="s">
+      <c r="G65" s="10"/>
+    </row>
+    <row r="66" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="50"/>
+      <c r="D66" s="18"/>
+      <c r="F66" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G61" s="11"/>
-    </row>
-    <row r="62" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="45"/>
-      <c r="F62" s="3" t="s">
+      <c r="G66" s="10"/>
+    </row>
+    <row r="67" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="50"/>
+      <c r="F67" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="45"/>
-      <c r="F63" s="3" t="s">
+    <row r="68" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="50"/>
+      <c r="F68" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="45"/>
-      <c r="F64" s="3" t="s">
+    <row r="69" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="50"/>
+      <c r="F69" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="45"/>
-      <c r="F65" s="3" t="s">
+    <row r="70" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="50"/>
+      <c r="F70" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="45"/>
-      <c r="F66" s="3" t="s">
+    <row r="71" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="50"/>
+      <c r="F71" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="45"/>
-      <c r="F67" s="3" t="s">
+    <row r="72" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="50"/>
+      <c r="F72" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="45"/>
-      <c r="F68" s="3" t="s">
+    <row r="73" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="50"/>
+      <c r="F73" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="45"/>
-      <c r="F69" s="3" t="s">
+    <row r="74" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="50"/>
+      <c r="F74" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="45"/>
-      <c r="F70" s="3" t="s">
+    <row r="75" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="50"/>
+      <c r="F75" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="45"/>
-      <c r="F72" s="3" t="s">
+    <row r="77" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="50"/>
+      <c r="F77" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="45"/>
-      <c r="F74" s="59" t="s">
+    <row r="79" spans="2:7" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="50"/>
+      <c r="F79" s="39" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="63"/>
-      <c r="F75" s="59"/>
-    </row>
-    <row r="76" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="45"/>
-      <c r="F76" s="3" t="s">
+    <row r="80" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="59"/>
+      <c r="F80" s="39"/>
+    </row>
+    <row r="81" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="50"/>
+      <c r="F81" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="45"/>
-      <c r="F77" s="3" t="s">
+    <row r="82" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="50"/>
+      <c r="F82" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="45"/>
-      <c r="F78" s="3" t="s">
+    <row r="83" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="50"/>
+      <c r="F83" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="45"/>
-      <c r="F79" s="3" t="s">
+    <row r="84" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="50"/>
+      <c r="F84" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="2:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="61" t="s">
+    <row r="86" spans="2:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="F81" s="3" t="s">
+      <c r="F86" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="82" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="62"/>
-    </row>
-    <row r="83" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F83" s="37" t="s">
+    <row r="87" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="61"/>
+    </row>
+    <row r="88" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F88" s="24" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F84" s="37"/>
-    </row>
-    <row r="85" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="45"/>
-      <c r="F85" s="3" t="s">
+    <row r="89" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F89" s="24"/>
+    </row>
+    <row r="90" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="50"/>
+      <c r="F90" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="45"/>
-      <c r="F86" s="3" t="s">
+    <row r="91" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="50"/>
+      <c r="F91" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="45"/>
-      <c r="F87" s="3" t="s">
+    <row r="92" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="50"/>
+      <c r="F92" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="45"/>
-      <c r="F88" s="3" t="s">
+    <row r="93" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="50"/>
+      <c r="F93" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="2:6" ht="363" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="45"/>
-      <c r="F90" s="59" t="s">
+    <row r="95" spans="2:6" ht="363" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="50"/>
+      <c r="F95" s="39" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="45"/>
-      <c r="F93" s="3" t="s">
+    <row r="98" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="50"/>
+      <c r="F98" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="95" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="60" t="s">
+    <row r="100" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="F95" s="3" t="s">
+      <c r="F100" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="45"/>
-      <c r="F97" s="3" t="s">
+    <row r="102" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="99" spans="2:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="60" t="s">
+    <row r="104" spans="2:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="F99" s="3" t="s">
+      <c r="F104" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="101" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="45"/>
-      <c r="F101" s="3" t="s">
+    <row r="106" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="50"/>
+      <c r="F106" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="103" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="45"/>
-      <c r="F103" s="3" t="s">
+    <row r="108" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="50"/>
+      <c r="F108" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="104" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="45"/>
-      <c r="F104" s="3" t="s">
+    <row r="109" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="50"/>
+      <c r="F109" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="105" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="45"/>
-      <c r="F105" s="3" t="s">
+    <row r="110" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="50"/>
+      <c r="F110" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="107" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="45"/>
-      <c r="F107" s="3" t="s">
+    <row r="112" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="50"/>
+      <c r="F112" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="108" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="45"/>
-      <c r="F108" s="3" t="s">
+    <row r="113" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="50"/>
+      <c r="F113" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="109" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="45"/>
-      <c r="F109" s="3" t="s">
+    <row r="114" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="50"/>
+      <c r="F114" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="45"/>
-      <c r="F111" s="3" t="s">
+    <row r="116" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="50"/>
+      <c r="F116" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="112" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="45"/>
-      <c r="F112" s="3" t="s">
+    <row r="117" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="50"/>
+      <c r="F117" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="45"/>
-      <c r="F113" s="3" t="s">
+    <row r="118" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="50"/>
+      <c r="F118" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="115" spans="2:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F115" s="37" t="s">
+    <row r="120" spans="2:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F120" s="24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="45"/>
-      <c r="F116" s="3" t="s">
+    <row r="121" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="50"/>
+      <c r="F121" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F118" s="37" t="s">
+    <row r="123" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F123" s="24" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="119" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="45"/>
-      <c r="F119" s="3" t="s">
+    <row r="124" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="50"/>
+      <c r="F124" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="121" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="45"/>
-      <c r="F121" s="3" t="s">
+    <row r="126" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="50"/>
+      <c r="F126" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="122" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="63"/>
-    </row>
-    <row r="123" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="63"/>
-      <c r="F123" s="37" t="s">
+    <row r="127" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="59"/>
+    </row>
+    <row r="128" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="59"/>
+      <c r="F128" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="124" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="63"/>
-      <c r="F124" s="37"/>
-    </row>
-    <row r="125" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="45"/>
-      <c r="F125" s="3" t="s">
+    <row r="129" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="59"/>
+      <c r="F129" s="24"/>
+    </row>
+    <row r="130" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="50"/>
+      <c r="F130" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="126" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="45"/>
-      <c r="F126" s="3" t="s">
+    <row r="131" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="50"/>
+      <c r="F131" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="127" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="45"/>
-      <c r="F127" s="3" t="s">
+    <row r="132" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="50"/>
+      <c r="F132" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="128" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="45"/>
-      <c r="F128" s="28" t="s">
+    <row r="133" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="50"/>
+      <c r="F133" s="21" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="129" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="45"/>
-      <c r="F129" s="3" t="s">
+    <row r="134" spans="2:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="F134" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F131" s="37" t="s">
+    <row r="136" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F136" s="24" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="132" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="45"/>
-      <c r="F132" s="3" t="s">
+    <row r="137" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="50"/>
+      <c r="F137" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="133" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="45"/>
-      <c r="F133" s="3" t="s">
+    <row r="138" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="50"/>
+      <c r="F138" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="134" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="45"/>
-    </row>
-    <row r="135" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="63"/>
-      <c r="F135" s="37" t="s">
+    <row r="139" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="50"/>
+    </row>
+    <row r="140" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="59"/>
+      <c r="F140" s="24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="136" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="63"/>
-    </row>
-    <row r="137" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="45"/>
-      <c r="F137" s="3" t="s">
+    <row r="141" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="59"/>
+    </row>
+    <row r="142" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="50"/>
+      <c r="F142" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="138" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="45"/>
-      <c r="F138" s="3" t="s">
+    <row r="143" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="50"/>
+      <c r="F143" s="3" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2151,9 +2147,9 @@
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F8 F11:F21 F23:F59">
+  <conditionalFormatting sqref="F6:F8 F11:F22 F24:F64">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>G6&gt;0</formula>
     </cfRule>
@@ -2185,7 +2181,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G59</xm:sqref>
+          <xm:sqref>G64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="3" id="{5EA8F3C7-7277-4F9C-B8C1-FC320B894E31}">
@@ -2204,7 +2200,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G60</xm:sqref>
+          <xm:sqref>G65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="2" id="{7ABC33D3-F1CF-4DF1-9FD2-C8CA715BB922}">
@@ -2223,7 +2219,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G61</xm:sqref>
+          <xm:sqref>G66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="41" id="{4B4E161B-C38F-4155-87F1-3F2FD6CA6AE1}">
@@ -2242,7 +2238,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G6:G58</xm:sqref>
+          <xm:sqref>G6:G63</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2472,21 +2468,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2509,14 +2505,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47CA8A17-D51D-491F-A5D8-2956C1CB93B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54D9BAC-15F5-4442-AF19-0D8B34179C0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2524,4 +2512,12 @@
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47CA8A17-D51D-491F-A5D8-2956C1CB93B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>